<commit_message>
Actualización Plan de Calidad
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Calidad/Plan_calidad.xlsx
+++ b/qualtcom/Organizacional/Calidad/Plan_calidad.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayra\escuela1\qualtcom\Organizacional\Calidad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\qtp\qualtcom\Organizacional\Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>Plan de calidad</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Mayra Tejeda</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Se deberá enviar la notificación que permita enterar, si no se realizó lo estipulado en la fecha límite a la persona responsable con copia a Dirección.</t>
   </si>
 </sst>
 </file>
@@ -257,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -280,6 +286,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,37 +643,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E31"/>
+  <dimension ref="B3:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:D23"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5"/>
     <col min="2" max="2" width="31.875"/>
     <col min="3" max="3" width="26.375"/>
     <col min="4" max="4" width="21.375"/>
-    <col min="5" max="5" width="13.25"/>
-    <col min="6" max="1025" width="10.5"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.625" customWidth="1"/>
+    <col min="7" max="1026" width="10.5"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E3" s="16"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
@@ -668,9 +686,10 @@
       <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E5" s="18"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
@@ -680,8 +699,9 @@
       <c r="D6" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
@@ -691,8 +711,9 @@
       <c r="D7" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E7" s="19"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>10</v>
       </c>
@@ -702,8 +723,9 @@
       <c r="D8" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>11</v>
       </c>
@@ -713,8 +735,9 @@
       <c r="D9" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E9" s="19"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
@@ -724,8 +747,9 @@
       <c r="D10" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>14</v>
       </c>
@@ -735,15 +759,17 @@
       <c r="D11" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E11" s="19"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="11"/>
       <c r="C16" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E16" s="16"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>16</v>
       </c>
@@ -753,8 +779,9 @@
       <c r="D17" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>17</v>
       </c>
@@ -764,8 +791,9 @@
       <c r="D18" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E18" s="19"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>18</v>
       </c>
@@ -775,8 +803,9 @@
       <c r="D19" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E19" s="19"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
         <v>19</v>
       </c>
@@ -786,8 +815,9 @@
       <c r="D20" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E20" s="19"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>20</v>
       </c>
@@ -797,8 +827,9 @@
       <c r="D21" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E21" s="19"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>21</v>
       </c>
@@ -808,8 +839,9 @@
       <c r="D22" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E22" s="19"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>22</v>
       </c>
@@ -819,8 +851,9 @@
       <c r="D23" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E23" s="19"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
         <v>23</v>
       </c>
@@ -830,16 +863,18 @@
       <c r="D24" s="10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E24" s="19"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="11"/>
       <c r="C28" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="13"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E28" s="13"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
         <v>25</v>
       </c>
@@ -852,8 +887,11 @@
       <c r="E29" s="15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F29" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
         <v>16</v>
       </c>
@@ -866,8 +904,11 @@
       <c r="E30" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F30" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>2</v>
       </c>
@@ -879,6 +920,9 @@
       </c>
       <c r="E31" s="10" t="s">
         <v>30</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>